<commit_message>
res mob data updates and texT
</commit_message>
<xml_diff>
--- a/data/residential-mobility/individual-model-scenarios/case-study-data.xlsx
+++ b/data/residential-mobility/individual-model-scenarios/case-study-data.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t xml:space="preserve">Cooksville</t>
   </si>
@@ -69,156 +70,156 @@
     <t xml:space="preserve">Single</t>
   </si>
   <si>
+    <t xml:space="preserve">age_10_to_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attached</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_15_to_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apt small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_20_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apt large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_25_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedrooms avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_30_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_35_39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_40_44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Dwellings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_45_49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleted Dwellings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_50_54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_55_59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_60_64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_65_69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_70_74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_75_79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_80_84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_85_100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedroom 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedroom 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low_inc_yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bedroom 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low_inc_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">married_yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">married_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existing_avgbedrooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existing_singledetached</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0209</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.1941</t>
   </si>
   <si>
-    <t xml:space="preserve">age_10_to_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attached</t>
+    <t xml:space="preserve">existing_rowtownsemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0923</t>
   </si>
   <si>
     <t xml:space="preserve">0.3117</t>
   </si>
   <si>
-    <t xml:space="preserve">age_15_to_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apt small</t>
+    <t xml:space="preserve">existing_aptsmall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7374</t>
   </si>
   <si>
     <t xml:space="preserve">0.3874</t>
   </si>
   <si>
-    <t xml:space="preserve">age_20_24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apt large</t>
+    <t xml:space="preserve">existing_aptlarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1495</t>
   </si>
   <si>
     <t xml:space="preserve">0.0837</t>
   </si>
   <si>
-    <t xml:space="preserve">age_25_29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedrooms avg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_30_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_35_39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scenario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_40_44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Dwellings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_45_49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deleted Dwellings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_50_54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_55_59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_60_64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_65_69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_70_74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_75_79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_80_84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age_85_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex_m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedroom 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex_f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedroom 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low_inc_yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedroom 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low_inc_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">married_yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">married_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existing_avgbedrooms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existing_singledetached</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existing_rowtownsemi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0923</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existing_aptsmall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7374</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existing_aptlarge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1495</t>
-  </si>
-  <si>
     <t xml:space="preserve">scenario1_totaldwellings</t>
   </si>
   <si>
@@ -328,6 +329,24 @@
   </si>
   <si>
     <t xml:space="preserve">2021S051235300060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low income population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario A low-income out movers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario B low-Income out movers</t>
   </si>
 </sst>
 </file>
@@ -445,7 +464,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -566,10 +585,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -596,10 +611,6 @@
     </xf>
     <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -685,11 +696,11 @@
   </sheetPr>
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.96"/>
@@ -796,7 +807,7 @@
         <v>12</v>
       </c>
       <c r="K4" s="13" t="n">
-        <v>759</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,14 +834,14 @@
       <c r="J5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>15</v>
+      <c r="K5" s="14" t="n">
+        <v>0.4124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>0.0471</v>
@@ -849,16 +860,16 @@
       </c>
       <c r="H6" s="11"/>
       <c r="J6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="K6" s="14" t="n">
+        <v>0.1975</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>0.047</v>
@@ -877,16 +888,16 @@
       </c>
       <c r="H7" s="11"/>
       <c r="J7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="K7" s="14" t="n">
+        <v>0.1541</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>0.0692</v>
@@ -905,16 +916,16 @@
       </c>
       <c r="H8" s="11"/>
       <c r="J8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="K8" s="14" t="n">
+        <v>0.2364</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>0.0902</v>
@@ -933,16 +944,16 @@
       </c>
       <c r="H9" s="11"/>
       <c r="J9" s="12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K9" s="13" t="n">
-        <v>2.506</v>
+        <v>2.859</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>0.0965</v>
@@ -969,7 +980,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>0.086</v>
@@ -988,13 +999,13 @@
       </c>
       <c r="H11" s="11"/>
       <c r="J11" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>0.0644</v>
@@ -1013,16 +1024,16 @@
       </c>
       <c r="H12" s="11"/>
       <c r="J12" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K12" s="16" t="n">
-        <v>10498</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0.0539</v>
@@ -1041,16 +1052,16 @@
       </c>
       <c r="H13" s="11"/>
       <c r="J13" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K13" s="16" t="n">
-        <v>0</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>0.0481</v>
@@ -1069,17 +1080,17 @@
       </c>
       <c r="H14" s="11"/>
       <c r="J14" s="17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K14" s="18" t="n">
         <f aca="false">K12+K4-K13</f>
-        <v>11257</v>
+        <v>3732</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>0.0581</v>
@@ -1098,19 +1109,19 @@
       </c>
       <c r="H15" s="11"/>
       <c r="L15" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>0.0604</v>
@@ -1131,30 +1142,28 @@
       <c r="J16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="19" t="n">
-        <v>0</v>
-      </c>
+      <c r="K16" s="19"/>
       <c r="L16" s="3" t="n">
         <f aca="false">K$12*K16</f>
         <v>0</v>
       </c>
       <c r="M16" s="3" t="n">
         <f aca="false">K5*(K$4-K$13)</f>
-        <v>147.3219</v>
+        <v>565.4004</v>
       </c>
       <c r="N16" s="3" t="n">
         <f aca="false">SUM(L16:M16)</f>
-        <v>147.3219</v>
+        <v>565.4004</v>
       </c>
       <c r="O16" s="20" t="n">
         <f aca="false">N16/N$20</f>
-        <v>0.0131075520475521</v>
+        <v>0.412235105957617</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>0.0536</v>
@@ -1173,32 +1182,30 @@
       </c>
       <c r="H17" s="11"/>
       <c r="J17" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="19" t="n">
-        <v>0</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="K17" s="19"/>
       <c r="L17" s="3" t="n">
         <f aca="false">K$12*K17</f>
         <v>0</v>
       </c>
       <c r="M17" s="3" t="n">
         <f aca="false">K6*(K$4-K$13)</f>
-        <v>236.5803</v>
+        <v>270.7725</v>
       </c>
       <c r="N17" s="3" t="n">
         <f aca="false">SUM(L17:M17)</f>
-        <v>236.5803</v>
+        <v>270.7725</v>
       </c>
       <c r="O17" s="20" t="n">
         <f aca="false">N17/N$20</f>
-        <v>0.0210490673530242</v>
+        <v>0.197421031587365</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>0.0422</v>
@@ -1217,32 +1224,30 @@
       </c>
       <c r="H18" s="11"/>
       <c r="J18" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="19" t="n">
-        <v>0.42</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="K18" s="19"/>
       <c r="L18" s="3" t="n">
         <f aca="false">K$12*K18</f>
-        <v>4409.16</v>
+        <v>0</v>
       </c>
       <c r="M18" s="3" t="n">
         <f aca="false">K7*(K$4-K$13)</f>
-        <v>294.0366</v>
+        <v>211.2711</v>
       </c>
       <c r="N18" s="3" t="n">
         <f aca="false">SUM(L18:M18)</f>
-        <v>4703.1966</v>
+        <v>211.2711</v>
       </c>
       <c r="O18" s="20" t="n">
         <f aca="false">N18/N$20</f>
-        <v>0.418453700531763</v>
+        <v>0.154038384646142</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>0.0341</v>
@@ -1261,32 +1266,30 @@
       </c>
       <c r="H19" s="11"/>
       <c r="J19" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="19" t="n">
-        <v>0.58</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K19" s="19"/>
       <c r="L19" s="3" t="n">
         <f aca="false">K$12*K19</f>
-        <v>6088.84</v>
+        <v>0</v>
       </c>
       <c r="M19" s="3" t="n">
         <f aca="false">K8*(K$4-K$13)</f>
-        <v>63.5283</v>
+        <v>324.1044</v>
       </c>
       <c r="N19" s="3" t="n">
         <f aca="false">SUM(L19:M19)</f>
-        <v>6152.3683</v>
+        <v>324.1044</v>
       </c>
       <c r="O19" s="20" t="n">
         <f aca="false">N19/N$20</f>
-        <v>0.547389680067661</v>
+        <v>0.236305477808876</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>0.0204</v>
@@ -1305,23 +1308,23 @@
       </c>
       <c r="H20" s="11"/>
       <c r="J20" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K20" s="3" t="n">
         <f aca="false">SUM(K16:K19)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="3" t="n">
         <f aca="false">SUM(L16:L19)</f>
-        <v>10498</v>
+        <v>0</v>
       </c>
       <c r="M20" s="3" t="n">
         <f aca="false">SUM(M16:M19)</f>
-        <v>741.4671</v>
+        <v>1371.5484</v>
       </c>
       <c r="N20" s="3" t="n">
         <f aca="false">SUM(N16:N19)</f>
-        <v>11239.4671</v>
+        <v>1371.5484</v>
       </c>
       <c r="O20" s="3" t="n">
         <f aca="false">SUM(O16:O19)</f>
@@ -1331,7 +1334,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>0.0217</v>
@@ -1353,7 +1356,7 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>0.4849</v>
@@ -1371,20 +1374,18 @@
         <v>0.5285</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="K22" s="16" t="n">
-        <v>0.5</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K22" s="16"/>
       <c r="L22" s="3" t="n">
         <f aca="false">K22*K$12*1</f>
-        <v>5249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>0.5151</v>
@@ -1402,20 +1403,18 @@
         <v>0.4715</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="K23" s="16" t="n">
-        <v>0.4</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="K23" s="16"/>
       <c r="L23" s="3" t="n">
         <f aca="false">K23*K$12*2</f>
-        <v>8398.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>0.1291</v>
@@ -1433,20 +1432,18 @@
         <v>0.152</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="K24" s="16" t="n">
-        <v>0.1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="K24" s="16"/>
       <c r="L24" s="3" t="n">
         <f aca="false">K24*K$12*3</f>
-        <v>3149.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>0.8709</v>
@@ -1464,33 +1461,33 @@
         <v>0.848</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K25" s="3" t="n">
         <f aca="false">SUM(K22:K24)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="3" t="n">
         <f aca="false">SUM(L22:L24)</f>
-        <v>16796.8</v>
+        <v>0</v>
       </c>
       <c r="M25" s="3" t="n">
         <f aca="false">K9*(K4-K13)</f>
-        <v>1902.054</v>
+        <v>3919.689</v>
       </c>
       <c r="N25" s="3" t="n">
         <f aca="false">L25+M25</f>
-        <v>18698.854</v>
+        <v>3919.689</v>
       </c>
       <c r="O25" s="21" t="n">
         <f aca="false">N25/K14</f>
-        <v>1.6610867904415</v>
+        <v>1.05029180064309</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>0.479</v>
@@ -1511,7 +1508,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>0.521</v>
@@ -1538,10 +1535,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>2.38</v>
@@ -1569,7 +1566,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C30" s="25" t="n">
         <v>0.0717</v>
@@ -1581,10 +1578,10 @@
         <v>0.4124</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="28"/>
@@ -1596,7 +1593,7 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" s="25" t="n">
         <v>0.1687</v>
@@ -1608,10 +1605,10 @@
         <v>0.1975</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="H31" s="27"/>
       <c r="I31" s="28"/>
@@ -1623,7 +1620,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32" s="25" t="n">
         <v>0.0782</v>
@@ -1635,10 +1632,10 @@
         <v>0.1541</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="28"/>
@@ -1648,7 +1645,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="25" t="n">
         <v>0.6814</v>
@@ -1660,24 +1657,21 @@
         <v>0.2364</v>
       </c>
       <c r="F33" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="26" t="s">
         <v>64</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>24</v>
       </c>
       <c r="H33" s="27"/>
       <c r="I33" s="28"/>
       <c r="J33" s="28"/>
       <c r="K33" s="29"/>
-      <c r="M33" s="30"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="31"/>
+      <c r="C34" s="30"/>
       <c r="I34" s="28"/>
       <c r="J34" s="28"/>
       <c r="K34" s="29"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -1686,11 +1680,14 @@
       <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="32" t="n">
+      <c r="C35" s="31" t="n">
         <v>37074</v>
       </c>
       <c r="D35" s="9" t="n">
         <v>10027</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>3732</v>
       </c>
       <c r="F35" s="3" t="n">
         <v>19941</v>
@@ -1704,7 +1701,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>66</v>
@@ -1714,6 +1711,9 @@
       </c>
       <c r="D36" s="4" t="n">
         <v>1.761</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>2.309</v>
       </c>
       <c r="F36" s="26" t="s">
         <v>67</v>
@@ -1738,10 +1738,13 @@
       <c r="D37" s="4" t="n">
         <v>0.0772112653874599</v>
       </c>
-      <c r="F37" s="33" t="n">
+      <c r="E37" s="3" t="n">
+        <v>0.218033388885502</v>
+      </c>
+      <c r="F37" s="32" t="n">
         <v>0.0134975034634817</v>
       </c>
-      <c r="G37" s="34" t="n">
+      <c r="G37" s="33" t="n">
         <v>0.0125546306231495</v>
       </c>
       <c r="I37" s="28"/>
@@ -1759,10 +1762,13 @@
       <c r="D38" s="4" t="n">
         <v>0.156096914336726</v>
       </c>
-      <c r="F38" s="33" t="n">
+      <c r="E38" s="3" t="n">
+        <v>0.591603655087141</v>
+      </c>
+      <c r="F38" s="32" t="n">
         <v>0.0596085918506873</v>
       </c>
-      <c r="G38" s="34" t="n">
+      <c r="G38" s="33" t="n">
         <v>0.0201611456220283</v>
       </c>
       <c r="I38" s="28"/>
@@ -1780,10 +1786,13 @@
       <c r="D39" s="4" t="n">
         <v>0.108046292665342</v>
       </c>
-      <c r="F39" s="33" t="n">
+      <c r="E39" s="3" t="n">
+        <v>0.0946148442836947</v>
+      </c>
+      <c r="F39" s="32" t="n">
         <v>0.529341199612307</v>
       </c>
-      <c r="G39" s="34" t="n">
+      <c r="G39" s="33" t="n">
         <v>0.0250575162463066</v>
       </c>
       <c r="I39" s="28"/>
@@ -1801,10 +1810,13 @@
       <c r="D40" s="4" t="n">
         <v>0.658645527610472</v>
       </c>
-      <c r="F40" s="35" t="n">
+      <c r="E40" s="3" t="n">
+        <v>0.095748111743662</v>
+      </c>
+      <c r="F40" s="34" t="n">
         <v>0.397552705073524</v>
       </c>
-      <c r="G40" s="34" t="n">
+      <c r="G40" s="33" t="n">
         <v>0.942226707508516</v>
       </c>
       <c r="I40" s="28"/>
@@ -1812,7 +1824,7 @@
       <c r="K40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="34"/>
+      <c r="C41" s="33"/>
       <c r="I41" s="28"/>
       <c r="J41" s="28"/>
       <c r="K41" s="29"/>
@@ -1824,11 +1836,14 @@
       <c r="B42" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="32" t="n">
+      <c r="C42" s="31" t="n">
         <v>30946.88</v>
       </c>
       <c r="D42" s="9" t="n">
         <v>9674</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>3874</v>
       </c>
       <c r="F42" s="3" t="n">
         <v>19824</v>
@@ -1842,7 +1857,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>73</v>
@@ -1852,6 +1867,12 @@
       </c>
       <c r="D43" s="4" t="n">
         <v>1.766</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>2.234</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>1.6284</v>
       </c>
       <c r="G43" s="3" t="n">
         <v>1.661</v>
@@ -1873,7 +1894,13 @@
       <c r="D44" s="4" t="n">
         <v>0.0794302878969151</v>
       </c>
-      <c r="G44" s="34" t="n">
+      <c r="E44" s="3" t="n">
+        <v>0.225270094911076</v>
+      </c>
+      <c r="F44" s="4" t="n">
+        <v>0.0135771597041978</v>
+      </c>
+      <c r="G44" s="4" t="n">
         <v>0.0131075520475521</v>
       </c>
       <c r="I44" s="28"/>
@@ -1891,7 +1918,13 @@
       <c r="D45" s="4" t="n">
         <v>0.156243397723382</v>
       </c>
-      <c r="G45" s="34" t="n">
+      <c r="E45" s="3" t="n">
+        <v>0.484645047939863</v>
+      </c>
+      <c r="F45" s="4" t="n">
+        <v>0.216794238836753</v>
+      </c>
+      <c r="G45" s="4" t="n">
         <v>0.0210490673530242</v>
       </c>
       <c r="I45" s="28"/>
@@ -1909,7 +1942,13 @@
       <c r="D46" s="4" t="n">
         <v>0.109513343773496</v>
       </c>
-      <c r="G46" s="34" t="n">
+      <c r="E46" s="3" t="n">
+        <v>0.177502250442991</v>
+      </c>
+      <c r="F46" s="4" t="n">
+        <v>0.52572972218981</v>
+      </c>
+      <c r="G46" s="4" t="n">
         <v>0.418453700531763</v>
       </c>
       <c r="I46" s="28"/>
@@ -1927,7 +1966,13 @@
       <c r="D47" s="4" t="n">
         <v>0.654812970606207</v>
       </c>
-      <c r="G47" s="34" t="n">
+      <c r="E47" s="3" t="n">
+        <v>0.11258260670607</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <v>0.243898879269239</v>
+      </c>
+      <c r="G47" s="4" t="n">
         <v>0.547389680067661</v>
       </c>
       <c r="I47" s="28"/>
@@ -1969,11 +2014,11 @@
   </sheetPr>
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.96"/>
@@ -2052,7 +2097,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>0.0471</v>
@@ -2064,7 +2109,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>0.047</v>
@@ -2076,7 +2121,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>0.0692</v>
@@ -2088,7 +2133,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>0.0902</v>
@@ -2100,7 +2145,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>0.0965</v>
@@ -2112,7 +2157,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>0.086</v>
@@ -2124,7 +2169,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>0.0644</v>
@@ -2136,7 +2181,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0.0539</v>
@@ -2148,7 +2193,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>0.0481</v>
@@ -2160,7 +2205,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>0.0581</v>
@@ -2172,7 +2217,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>0.0604</v>
@@ -2184,7 +2229,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>0.0536</v>
@@ -2196,7 +2241,7 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>0.0422</v>
@@ -2208,7 +2253,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>0.0341</v>
@@ -2220,7 +2265,7 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>0.0204</v>
@@ -2232,7 +2277,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>0.0217</v>
@@ -2244,7 +2289,7 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>0.4849</v>
@@ -2256,7 +2301,7 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>0.5151</v>
@@ -2268,7 +2313,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>0.1291</v>
@@ -2277,7 +2322,7 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>0.8709</v>
@@ -2286,7 +2331,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>0.479</v>
@@ -2298,7 +2343,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>0.521</v>
@@ -2322,19 +2367,19 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="M28" s="36" t="s">
+      <c r="M28" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="O28" s="36" t="s">
+      <c r="O28" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>2.38</v>
@@ -2350,10 +2395,10 @@
       <c r="L29" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="M29" s="37" t="s">
+      <c r="M29" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="O29" s="37" t="s">
+      <c r="O29" s="36" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2362,9 +2407,9 @@
         <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="31" t="n">
+        <v>53</v>
+      </c>
+      <c r="C30" s="30" t="n">
         <v>0.0717</v>
       </c>
       <c r="D30" s="0" t="n">
@@ -2388,19 +2433,19 @@
       <c r="L30" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="M30" s="37" t="s">
+      <c r="M30" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="O30" s="37" t="s">
+      <c r="O30" s="36" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="31" t="n">
+        <v>56</v>
+      </c>
+      <c r="C31" s="30" t="n">
         <v>0.1687</v>
       </c>
       <c r="D31" s="0" t="n">
@@ -2424,19 +2469,19 @@
       <c r="L31" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="M31" s="37" t="s">
+      <c r="M31" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="O31" s="37" t="s">
+      <c r="O31" s="36" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="31" t="n">
+        <v>59</v>
+      </c>
+      <c r="C32" s="30" t="n">
         <v>0.0782</v>
       </c>
       <c r="D32" s="0" t="n">
@@ -2458,11 +2503,11 @@
       <c r="J32" s="28"/>
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
-      <c r="M32" s="38" t="n">
+      <c r="M32" s="37" t="n">
         <f aca="false">M29*(C35-C28)</f>
         <v>11884.4</v>
       </c>
-      <c r="N32" s="38" t="n">
+      <c r="N32" s="37" t="n">
         <f aca="false">M32*1</f>
         <v>11884.4</v>
       </c>
@@ -2470,9 +2515,9 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="31" t="n">
+        <v>62</v>
+      </c>
+      <c r="C33" s="30" t="n">
         <v>0.6814</v>
       </c>
       <c r="D33" s="0" t="n">
@@ -2494,17 +2539,17 @@
       <c r="J33" s="28"/>
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
-      <c r="M33" s="38" t="n">
+      <c r="M33" s="37" t="n">
         <f aca="false">M30*(C35-C28)</f>
         <v>8913.3</v>
       </c>
-      <c r="N33" s="39" t="n">
+      <c r="N33" s="37" t="n">
         <f aca="false">M33*2</f>
         <v>17826.6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="31"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="0"/>
       <c r="E34" s="0"/>
       <c r="F34" s="0"/>
@@ -2514,11 +2559,11 @@
       <c r="J34" s="28"/>
       <c r="K34" s="28"/>
       <c r="L34" s="28"/>
-      <c r="M34" s="39" t="n">
+      <c r="M34" s="37" t="n">
         <f aca="false">M31*(C35-C28)</f>
         <v>8913.3</v>
       </c>
-      <c r="N34" s="39" t="n">
+      <c r="N34" s="37" t="n">
         <f aca="false">M34*3</f>
         <v>26739.9</v>
       </c>
@@ -2530,7 +2575,7 @@
       <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="32" t="n">
+      <c r="C35" s="31" t="n">
         <v>37074</v>
       </c>
       <c r="D35" s="0" t="n">
@@ -2544,18 +2589,18 @@
       <c r="J35" s="28"/>
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
-      <c r="M35" s="38" t="n">
+      <c r="M35" s="37" t="n">
         <f aca="false">SUM(M32:M34)</f>
         <v>29711</v>
       </c>
-      <c r="N35" s="38" t="n">
+      <c r="N35" s="37" t="n">
         <f aca="false">SUM(N32:N34)</f>
         <v>56450.9</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>66</v>
@@ -2567,12 +2612,12 @@
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
       <c r="G36" s="0"/>
-      <c r="H36" s="38"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="3"/>
       <c r="J36" s="28"/>
       <c r="K36" s="28"/>
       <c r="L36" s="28"/>
-      <c r="N36" s="38" t="n">
+      <c r="N36" s="37" t="n">
         <f aca="false">C28*C29</f>
         <v>17523.94</v>
       </c>
@@ -2584,7 +2629,7 @@
       <c r="B37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="34" t="n">
+      <c r="C37" s="33" t="n">
         <v>0.0142398203592814</v>
       </c>
       <c r="D37" s="0"/>
@@ -2607,7 +2652,7 @@
         <v>0.0142398203592814</v>
       </c>
       <c r="L37" s="28"/>
-      <c r="N37" s="38" t="n">
+      <c r="N37" s="37" t="n">
         <f aca="false">N35+N36</f>
         <v>73974.84</v>
       </c>
@@ -2617,7 +2662,7 @@
       <c r="B38" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="34" t="n">
+      <c r="C38" s="33" t="n">
         <v>0.0335042914171657</v>
       </c>
       <c r="D38" s="0"/>
@@ -2640,7 +2685,7 @@
         <v>0.0335042914171657</v>
       </c>
       <c r="L38" s="28"/>
-      <c r="N38" s="38" t="n">
+      <c r="N38" s="37" t="n">
         <f aca="false">N37/C35</f>
         <v>1.99532934131737</v>
       </c>
@@ -2650,7 +2695,7 @@
       <c r="B39" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="34" t="n">
+      <c r="C39" s="33" t="n">
         <v>0.0636145708582834</v>
       </c>
       <c r="D39" s="0"/>
@@ -2679,7 +2724,7 @@
       <c r="B40" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="34" t="n">
+      <c r="C40" s="33" t="n">
         <v>0.888641317365269</v>
       </c>
       <c r="D40" s="0"/>
@@ -2704,7 +2749,7 @@
       <c r="L40" s="28"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="34"/>
+      <c r="C41" s="33"/>
       <c r="D41" s="0"/>
       <c r="E41" s="0"/>
       <c r="F41" s="0"/>
@@ -2722,7 +2767,7 @@
       <c r="B42" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="32" t="n">
+      <c r="C42" s="31" t="n">
         <v>30946.88</v>
       </c>
       <c r="D42" s="0" t="n">
@@ -2742,7 +2787,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>73</v>
@@ -2767,7 +2812,7 @@
       <c r="B44" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C44" s="34" t="n">
+      <c r="C44" s="33" t="n">
         <v>0.0142398203592814</v>
       </c>
       <c r="D44" s="0"/>
@@ -2796,7 +2841,7 @@
       <c r="B45" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="34" t="n">
+      <c r="C45" s="33" t="n">
         <v>0.0335042914171657</v>
       </c>
       <c r="D45" s="0"/>
@@ -2825,7 +2870,7 @@
       <c r="B46" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="34" t="n">
+      <c r="C46" s="33" t="n">
         <v>0.0855050277822733</v>
       </c>
       <c r="D46" s="0"/>
@@ -2854,7 +2899,7 @@
       <c r="B47" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="34" t="n">
+      <c r="C47" s="33" t="n">
         <v>0.701483557209905</v>
       </c>
       <c r="D47" s="0"/>
@@ -2890,7 +2935,7 @@
         <v>30946.88</v>
       </c>
       <c r="K48" s="28"/>
-      <c r="L48" s="36"/>
+      <c r="L48" s="35"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F49" s="23"/>
@@ -2925,11 +2970,11 @@
   </sheetPr>
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.57"/>
   </cols>
@@ -3855,4 +3900,64 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B5:D10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.4"/>
+  </cols>
+  <sheetData>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
res mob sim mod
</commit_message>
<xml_diff>
--- a/data/residential-mobility/individual-model-scenarios/case-study-data.xlsx
+++ b/data/residential-mobility/individual-model-scenarios/case-study-data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
   <si>
     <t xml:space="preserve">Cooksville</t>
   </si>
@@ -257,6 +257,42 @@
   </si>
   <si>
     <t xml:space="preserve">scenario2_aptlarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario1_totaldwellings_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario1_avgbedrooms_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario1_singledetached_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario1_rowtownsemi_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario1_aptsmall_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario1_aptlarge_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario2_totaldwellings_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario2_avgbedrooms_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario2_singledetached_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario2_rowtownsemi_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario2_aptsmall_percchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario2_aptlarge_percchange</t>
   </si>
   <si>
     <t xml:space="preserve">Scenario 2 (Optimized)</t>
@@ -694,13 +730,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.96"/>
@@ -1985,9 +2021,252 @@
       <c r="K48" s="22"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
+      <c r="B49" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="9" t="n">
+        <v>403.517587939699</v>
+      </c>
+      <c r="D49" s="9" t="n">
+        <v>372.080979284369</v>
+      </c>
+      <c r="E49" s="9" t="n">
+        <v>112.166003411029</v>
+      </c>
+      <c r="F49" s="31" t="n">
+        <v>48.5584444609998</v>
+      </c>
+      <c r="G49" s="31" t="n">
+        <v>1448.35309617918</v>
+      </c>
       <c r="H49" s="22"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="9" t="n">
+        <v>-35.7142857142857</v>
+      </c>
+      <c r="D50" s="9" t="n">
+        <v>-32.5287356321839</v>
+      </c>
+      <c r="E50" s="9" t="n">
+        <v>-19.2374956278419</v>
+      </c>
+      <c r="F50" s="9" t="n">
+        <v>-0.74224021592442</v>
+      </c>
+      <c r="G50" s="9" t="n">
+        <v>-33.8188347964884</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="9" t="n">
+        <v>-12.6578840146681</v>
+      </c>
+      <c r="D51" s="9" t="n">
+        <v>-2.48804233307282</v>
+      </c>
+      <c r="E51" s="9" t="n">
+        <v>12.1708844083405</v>
+      </c>
+      <c r="F51" s="9" t="n">
+        <v>-4.05894169177998</v>
+      </c>
+      <c r="G51" s="9" t="n">
+        <v>0.149413687478176</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="9" t="n">
+        <v>-12.6578840146679</v>
+      </c>
+      <c r="D52" s="9" t="n">
+        <v>319.649112661446</v>
+      </c>
+      <c r="E52" s="9" t="n">
+        <v>535.535104319977</v>
+      </c>
+      <c r="F52" s="9" t="n">
+        <v>-4.0589416917797</v>
+      </c>
+      <c r="G52" s="9" t="n">
+        <v>0.149413687478025</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="9" t="n">
+        <v>306.65833487615</v>
+      </c>
+      <c r="D53" s="9" t="n">
+        <v>67.7296930269655</v>
+      </c>
+      <c r="E53" s="9" t="n">
+        <v>30.2664073655311</v>
+      </c>
+      <c r="F53" s="9" t="n">
+        <v>6.6423992453538</v>
+      </c>
+      <c r="G53" s="9" t="n">
+        <v>0.149413687478062</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="9" t="n">
+        <v>561.461493204446</v>
+      </c>
+      <c r="D54" s="9" t="n">
+        <v>2029.68510736727</v>
+      </c>
+      <c r="E54" s="9" t="n">
+        <v>-14.0672834060686</v>
+      </c>
+      <c r="F54" s="9" t="n">
+        <v>295.048906066792</v>
+      </c>
+      <c r="G54" s="9" t="n">
+        <v>17330.1032242954</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="9" t="n">
+        <v>320.302594051338</v>
+      </c>
+      <c r="D56" s="9" t="n">
+        <v>355.461393596987</v>
+      </c>
+      <c r="E56" s="9" t="n">
+        <v>120.238772029562</v>
+      </c>
+      <c r="F56" s="9" t="n">
+        <v>47.6868062281159</v>
+      </c>
+      <c r="G56" s="9" t="n">
+        <v>1383.13570487484</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="9" t="n">
+        <v>-15.9770037850021</v>
+      </c>
+      <c r="D57" s="9" t="n">
+        <v>-32.3371647509579</v>
+      </c>
+      <c r="E57" s="9" t="n">
+        <v>-21.860790486184</v>
+      </c>
+      <c r="F57" s="9" t="n">
+        <v>9.87854251012146</v>
+      </c>
+      <c r="G57" s="9" t="n">
+        <v>-33.7190742218675</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="9" t="n">
+        <v>-12.6582226922109</v>
+      </c>
+      <c r="D58" s="9" t="n">
+        <v>-3.21714922595285</v>
+      </c>
+      <c r="E58" s="9" t="n">
+        <v>20.3036107618776</v>
+      </c>
+      <c r="F58" s="9" t="n">
+        <v>-4.05897826018926</v>
+      </c>
+      <c r="G58" s="9" t="n">
+        <v>0.155994050642836</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" s="9" t="n">
+        <v>-12.6582226922108</v>
+      </c>
+      <c r="D59" s="9" t="n">
+        <v>305.255328402163</v>
+      </c>
+      <c r="E59" s="9" t="n">
+        <v>440.443697359411</v>
+      </c>
+      <c r="F59" s="9" t="n">
+        <v>246.886768607318</v>
+      </c>
+      <c r="G59" s="9" t="n">
+        <v>0.155994050643039</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="9" t="n">
+        <v>455.700982445775</v>
+      </c>
+      <c r="D60" s="9" t="n">
+        <v>64.0220327936284</v>
+      </c>
+      <c r="E60" s="9" t="n">
+        <v>153.685124400053</v>
+      </c>
+      <c r="F60" s="9" t="n">
+        <v>5.29338704828814</v>
+      </c>
+      <c r="G60" s="9" t="n">
+        <v>1502.02277773789</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="9" t="n">
+        <v>422.233363603296</v>
+      </c>
+      <c r="D61" s="9" t="n">
+        <v>1942.75361738141</v>
+      </c>
+      <c r="E61" s="9" t="n">
+        <v>4.88601968203052</v>
+      </c>
+      <c r="F61" s="9" t="n">
+        <v>140.94077941064</v>
+      </c>
+      <c r="G61" s="9" t="n">
+        <v>9599.56008349296</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2018,7 +2297,7 @@
       <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.96"/>
@@ -2368,10 +2647,10 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="M28" s="35" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="O28" s="35" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,10 +2675,10 @@
         <v>1</v>
       </c>
       <c r="M29" s="36" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="O29" s="36" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,10 +2713,10 @@
         <v>2</v>
       </c>
       <c r="M30" s="36" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="O30" s="36" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2470,10 +2749,10 @@
         <v>3</v>
       </c>
       <c r="M31" s="36" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="O31" s="36" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,47 +3253,47 @@
       <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,7 +3301,7 @@
         <v>35300054</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>0.1317</v>
@@ -3064,7 +3343,7 @@
         <v>35300055</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>0.0737</v>
@@ -3106,7 +3385,7 @@
         <v>35300056</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>0.1549</v>
@@ -3148,7 +3427,7 @@
         <v>35300059</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>0.1742</v>
@@ -3190,7 +3469,7 @@
         <v>35300060</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>0.1061</v>
@@ -3913,7 +4192,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.4"/>
   </cols>
@@ -3925,30 +4204,30 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>